<commit_message>
Audit report spreadsheet updated
</commit_message>
<xml_diff>
--- a/SEO/Template-SEO-audit_Steve_20juilet2021.xlsx
+++ b/SEO/Template-SEO-audit_Steve_20juilet2021.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -100,7 +100,10 @@
     <t xml:space="preserve">Broken links at the bottom of the page are recognise as balck hat practice and the site will be punch down in google search</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove black hat links at the bottom of the page and don’t create fake links in the website</t>
+    <t xml:space="preserve">Don’t make black hat links at the bottom of the page and don’t create fake links in the website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove black hat links at the bottom of the page and remove create fake links in the website</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.greengeeks.com/blog/11-clever-ways-to-get-quality-backlinks-to-your-website/</t>
@@ -148,6 +151,9 @@
     <t xml:space="preserve">Color contrast must comply with WCAG 2.1 AA level requirements</t>
   </si>
   <si>
+    <t xml:space="preserve">Background color to change</t>
+  </si>
+  <si>
     <t xml:space="preserve">Visibility / Invisibility</t>
   </si>
   <si>
@@ -200,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">Article in text fomat is more responsive than an image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text should be html not image</t>
   </si>
   <si>
     <t xml:space="preserve">Change image to text in article with tags</t>
@@ -221,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -283,12 +292,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -338,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,10 +371,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,14 +454,14 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="59.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="59.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="56.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45.63"/>
@@ -627,7 +626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="43.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -640,22 +639,22 @@
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>26</v>
+      <c r="E11" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="5"/>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -664,10 +663,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -676,10 +675,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -688,10 +687,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -700,16 +699,16 @@
     </row>
     <row r="17" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -718,79 +717,78 @@
     </row>
     <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -809,7 +807,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E30" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -818,61 +816,64 @@
     </row>
     <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="8" t="s">
-        <v>61</v>
+      <c r="B36" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B18" r:id="rId1" location="general_guidelines" display="General guidelines"/>
-    <hyperlink ref="D23" r:id="rId2" location="state_prop_def" display="ARIA States"/>
+    <hyperlink ref="D23" r:id="rId2" location="state_prop_def" display="custom controls state changes must be provided via ARIA States "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Modification of SEO audit Modification of SEO audit spreedcheat
</commit_message>
<xml_diff>
--- a/SEO/Template-SEO-audit_Steve_20juilet2021.xlsx
+++ b/SEO/Template-SEO-audit_Steve_20juilet2021.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Details" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Summary" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -454,7 +455,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -883,4 +884,27 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>